<commit_message>
-fresh wind data manually collected
</commit_message>
<xml_diff>
--- a/inst/extdata/China fossil fuel imports from Russia - backup.xlsx
+++ b/inst/extdata/China fossil fuel imports from Russia - backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wind\Desktop\automation\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9B9CF8-8D8A-4CF4-BF24-78F82D77236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C89FE3-9812-41CF-8F2B-8130FDD94EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="11520" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,9 +541,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1" t="str">
+      <c r="A1" s="1">
         <f>[1]!edb()</f>
-        <v>Wind</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>

</xml_diff>